<commit_message>
added systematic way for training new models. Feature include: 1. randomize train test split (random new batch of data) 2. save the train-test dataframes in model folder 3. save csv of dataframes 4. save info about number of examples per label
</commit_message>
<xml_diff>
--- a/data/image_labels.xlsx
+++ b/data/image_labels.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="174">
   <si>
     <t xml:space="preserve">#</t>
   </si>
@@ -497,6 +497,51 @@
   </si>
   <si>
     <t xml:space="preserve">T596-1-14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D1b-40-0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D1b-42-0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T510-4-250</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T693-200-8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T693-200-10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T693-200-13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T703-75-8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T705-142-5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T704-2-200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T704-2-300</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T704-142-4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T704-142-5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T704-142-8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T704-142-13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T704-200-4</t>
   </si>
 </sst>
 </file>
@@ -690,16 +735,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I154"/>
+  <dimension ref="A1:I169"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A139" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B170" activeCellId="0" sqref="B170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.42"/>
@@ -2274,11 +2319,131 @@
         <v>10</v>
       </c>
     </row>
-    <row r="154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B154" s="0" t="s">
         <v>158</v>
       </c>
       <c r="C154" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B155" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="C155" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B156" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="C156" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B157" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="C157" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B158" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="C158" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B159" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="C159" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B160" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="C160" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B161" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="C161" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B162" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="C162" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B163" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="C163" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B164" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="C164" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B165" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="C165" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B166" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="C166" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B167" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="C167" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B168" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C168" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B169" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="C169" s="5" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>